<commit_message>
Casos de prueba manuales
</commit_message>
<xml_diff>
--- a/qa-testing/Planeación casos de prueba sprint II.xlsx
+++ b/qa-testing/Planeación casos de prueba sprint II.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
   <si>
     <t xml:space="preserve">Épica</t>
   </si>
@@ -137,7 +137,7 @@
     <r>
       <rPr>
         <b val="true"/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
@@ -148,7 +148,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
@@ -170,30 +170,29 @@
     <r>
       <rPr>
         <b val="true"/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Bloque header:
 </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Debe cubrir el 100 % del ancho de la pantalla.
-- Incluir alineado a la izquierda dentro del área de
-contenido:
+- Incluir alineado a la izquierda dentro del área de contenido:
   - Categoría del producto
   - Título del producto
-- Incluir alineado a la derecha dentro del área de
-contenido:
-- Flecha volver atrás: Implementar un ícono debajo
-del header que permita volver a la home.</t>
+- Incluir alineado a la derecha dentro del área de contenido:
+- Flecha volver atrás: Implementar un ícono debajo del header que permita volver a la home.</t>
     </r>
   </si>
   <si>
@@ -218,7 +217,7 @@
     <r>
       <rPr>
         <b val="true"/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
@@ -229,14 +228,13 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Debe cubrir el 100 % del ancho de la
-pantalla e incluir dentro del área de contenido:
+      <t xml:space="preserve">Debe cubrir el 100 % del ancho de la pantalla e incluir dentro del área de contenido:
 - Datos de ubicación.</t>
     </r>
   </si>
@@ -259,7 +257,7 @@
     <r>
       <rPr>
         <b val="true"/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
@@ -270,7 +268,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
@@ -339,7 +337,7 @@
     <r>
       <rPr>
         <b val="true"/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
@@ -350,14 +348,13 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="AnjaliOldLipi"/>
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Bloque que cubra el 100 % del
-contenedor que incluya:
+      <t xml:space="preserve">- Bloque que cubra el 100 % del contenedor que incluya:
 - Título
 - Texto de descripción del producto.</t>
     </r>
@@ -404,13 +401,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Bloque que cubra el 100 % del
-contenedor que incluya:
+    <t xml:space="preserve">Bloque que cubra el 100 % del contenedor que incluya:
 - Título subrayado.
-- Grilla de 4 columnas para desktop, 2 para
-tablet y 1 para phone con una enumeración de
-los atributos del producto junto a su ícono
-asociado.</t>
+- Grilla de 4 columnas para desktop, 2 para tablet y 1 para phone con una enumeración de los atributos del producto junto a su ícono
+Asociado. </t>
   </si>
   <si>
     <t xml:space="preserve">Como usuario quiero poder visualizar la
@@ -454,9 +448,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Bloque que cubra el 100 % del contenedor
-que incluya una grilla de 3 columnas para desktop, 2
-para tablet y 1 para phone con:
+    <t xml:space="preserve">Bloque que cubra el 100 % del contenedor que incluya una grilla de 3 columnas para desktop, 2 para tablet y 1 para phone con:
   - Normas: Título y descripción.  
   - Seguridad: Título y descripción.
   - Cancelación: Título y descripción.</t>
@@ -520,8 +512,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">El select de ciudades del buscador debe mostrar las
-ciudades almacenadas en la base de datos.</t>
+    <t xml:space="preserve">El select de ciudades del buscador debe mostrar las ciudades almacenadas en la base de datos. </t>
   </si>
   <si>
     <t xml:space="preserve">Como usuario quiero poder ﬁltrar por una
@@ -555,11 +546,94 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">- Las categorías que se ven en el home deben
-obtenerse de la base de datos.
-- Listar productos según categoría. Al clickear en una
-categoría, se deben obtener de la base de datos y
-mostrar los productos de esa categoría.</t>
+    <t xml:space="preserve">- Las categorías que se ven en el home deben obtenerse de la base de datos.
+- Listar productos según categoría. Al clickear en una categoría, se deben obtener de la base de datos y mostrar los productos de esa categoría.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserva
+de productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como usuario quiero poder visualizar las
+fechas disponibles en el detalle de producto y
+poder acceder a la sección de reservas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reservas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserva de productos – desktop</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="AnjaliOldLipi"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">En desktop:
+- Debe incluir un calendario alineado a la izquierda y que ocupe ⅔ partes de la grilla de contenido, que muestre 2 meses simultáneamente e indique tanto fechas disponibles como no disponibles.
+- El calendario solo debe permitir navegar entre distintos meses (su única ﬁnalidad es la visualización de disponibilidad).
+- Bloque de reserva debe ocupar ⅓ parte de la grilla de contenido:
+  - Alinearlo a la derecha del calendario.
+  - Debe incluir un texto.
+  - Debe incluir un </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="AnjaliOldLipi"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">botón de “Iniciar reserva”
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="AnjaliOldLipi"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(sin eventos).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">C-019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserva de productos – tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tablet:
+- Debe incluir un calendario al 100 % del ancho del contenedor que muestre 2 meses simultáneamente que indique tanto fechas disponibles como no disponibles.
+- El calendario solo debe permitir navegar entre distintos meses (su única ﬁnalidad es la visualización de disponibilidad).
+- Bloque de reserva con una grilla de 2 columnas:
+  - Debe incluir un texto.
+  - Debe incluir un botón de “Iniciar reserva”
+(sin eventos).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserva de productos – phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En phone:
+- Debe incluir un calendario al 100 % del ancho del contenedor que muestre un mes simultáneamente que indique tanto fechas disponibles como no disponibles.
+- El calendario solo debe permitir navegar entre distintos meses (su única ﬁnalidad es la visualización de disponibilidad).
+- Bloque de reserva:
+  - Debe incluir un texto al 100 % del ancho de la pantalla.
+  - Debe incluir un botón de “Iniciar reserva” (sin eventos) al 100 % del ancho de la pantalla.</t>
   </si>
 </sst>
 </file>
@@ -569,7 +643,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -614,17 +688,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="AnjaliOldLipi"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="AnjaliOldLipi"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -635,14 +703,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
       <name val="AnjaliOldLipi"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="AnjaliOldLipi"/>
       <family val="0"/>
     </font>
@@ -721,7 +788,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -758,7 +825,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -770,11 +837,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -786,11 +849,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -873,10 +932,10 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1016,11 +1075,11 @@
         <v>27</v>
       </c>
       <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="75.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
@@ -1085,7 +1144,7 @@
       <c r="H6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -1166,7 +1225,7 @@
       <c r="G8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>49</v>
       </c>
       <c r="I8" s="12" t="s">
@@ -1198,8 +1257,8 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15" t="s">
+      <c r="H9" s="13"/>
+      <c r="I9" s="12" t="s">
         <v>52</v>
       </c>
       <c r="J9" s="6" t="s">
@@ -1238,7 +1297,7 @@
       <c r="G10" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="14" t="s">
         <v>49</v>
       </c>
       <c r="I10" s="12" t="s">
@@ -1258,7 +1317,7 @@
       </c>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>28</v>
       </c>
@@ -1280,10 +1339,10 @@
       <c r="G11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="15" t="s">
         <v>63</v>
       </c>
       <c r="J11" s="6" t="s">
@@ -1322,10 +1381,10 @@
       <c r="G12" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="15" t="s">
         <v>69</v>
       </c>
       <c r="J12" s="6" t="s">
@@ -1367,7 +1426,7 @@
       <c r="H13" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="15" t="s">
         <v>76</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -1409,7 +1468,7 @@
       <c r="H14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="15" t="s">
         <v>80</v>
       </c>
       <c r="J14" s="6" t="s">
@@ -1427,7 +1486,9 @@
       <c r="N14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="82.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="B15" s="6" t="s">
         <v>81</v>
       </c>
@@ -1449,7 +1510,7 @@
       <c r="H15" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="15" t="s">
         <v>85</v>
       </c>
       <c r="J15" s="6" t="s">
@@ -1466,16 +1527,32 @@
       </c>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+    <row r="16" customFormat="false" ht="133.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="17"/>
+      <c r="I16" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="J16" s="6" t="s">
         <v>23</v>
       </c>
@@ -1490,16 +1567,32 @@
       </c>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+    <row r="17" customFormat="false" ht="117.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="H17" s="8"/>
-      <c r="I17" s="17"/>
+      <c r="I17" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="J17" s="6" t="s">
         <v>23</v>
       </c>
@@ -1514,16 +1607,32 @@
       </c>
       <c r="N17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+    <row r="18" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="H18" s="8"/>
-      <c r="I18" s="17"/>
+      <c r="I18" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="J18" s="6" t="s">
         <v>23</v>
       </c>
@@ -1547,19 +1656,11 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="I19" s="15"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
       <c r="N19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1571,19 +1672,11 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="I20" s="15"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
       <c r="N20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1595,19 +1688,11 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="I21" s="15"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
       <c r="N21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1619,19 +1704,11 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
       <c r="N22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1643,19 +1720,11 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="I23" s="15"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>